<commit_message>
added to micromouse schematic
</commit_message>
<xml_diff>
--- a/micromouse_bom.xlsx
+++ b/micromouse_bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\destroyorzss\Documents\micromouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyen37\Documents\micromouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18195"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="38400" windowHeight="18195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Nicholas Nguyen</t>
   </si>
@@ -60,12 +60,18 @@
   </si>
   <si>
     <t>Wires with Pre-Crimped Terminals 60-Piece 6-Color Assortment M-M 2"</t>
+  </si>
+  <si>
+    <t>9V Battery Clips w/ Bare Wires</t>
+  </si>
+  <si>
+    <t>ATMega328P-PU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -421,8 +427,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -470,6 +476,11 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>11</v>
@@ -485,11 +496,17 @@
         <v>9</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1"/>
-    <hyperlink ref="C11" r:id="rId2"/>
-    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C12" r:id="rId4" xr:uid="{D97027A7-F195-4A0C-9594-7E052F289AFC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gerber files and eagle files
</commit_message>
<xml_diff>
--- a/micromouse_bom.xlsx
+++ b/micromouse_bom.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyen37\Documents\micromouse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\destroyorzss\Documents\micromouse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="38400" windowHeight="18195" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="38400" windowHeight="18195"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nicholas Nguyen</t>
   </si>
@@ -66,12 +66,18 @@
   </si>
   <si>
     <t>ATMega328P-PU</t>
+  </si>
+  <si>
+    <t>Voltage Regulator</t>
+  </si>
+  <si>
+    <t>Slide Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -427,11 +433,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +487,16 @@
         <v>13</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>11</v>
@@ -503,10 +519,12 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="C11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C12" r:id="rId4" xr:uid="{D97027A7-F195-4A0C-9594-7E052F289AFC}"/>
+    <hyperlink ref="C10" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>